<commit_message>
Results from July 14, 2020 07:38:26 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-14.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-14.xlsx
@@ -2165,18 +2165,32 @@
           <t>Iowa</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="B36" s="2" t="n">
+        <v>44026</v>
+      </c>
+      <c r="C36" t="n">
+        <v>35865</v>
+      </c>
+      <c r="D36" t="n">
+        <v>757</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3078</v>
+      </c>
+      <c r="F36" t="n">
+        <v>36</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8.58</v>
+      </c>
+      <c r="H36" t="n">
+        <v>4.76</v>
+      </c>
       <c r="I36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2188,7 +2202,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>An error occurred. ... TypeError('list indices must be integers or slices, not str')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 14, 2020 09:06:32 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-14.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-14.xlsx
@@ -1260,21 +1260,39 @@
           <t>Maryland</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="B17" s="2" t="n">
+        <v>44026</v>
+      </c>
+      <c r="C17" t="n">
+        <v>74260</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3202</v>
+      </c>
+      <c r="E17" t="n">
+        <v>21525</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1301</v>
+      </c>
+      <c r="G17" t="n">
+        <v>35.07</v>
+      </c>
+      <c r="H17" t="n">
+        <v>40.87</v>
+      </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+      <c r="K17" t="n">
+        <v>61384</v>
+      </c>
+      <c r="L17" t="n">
+        <v>3183</v>
+      </c>
       <c r="M17" t="n">
         <v>1788090</v>
       </c>
@@ -1283,7 +1301,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>An error occurred. ... TypeError("'float' object is not iterable")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2187,7 @@
         <v>44026</v>
       </c>
       <c r="C36" t="n">
-        <v>35865</v>
+        <v>35866</v>
       </c>
       <c r="D36" t="n">
         <v>757</v>

</xml_diff>